<commit_message>
Updates to hook scripts for Marot et al 2020, Rodriguez et al 2022, and Curtis et al 2022
</commit_message>
<xml_diff>
--- a/data/primary_studies/Marot_et_al_2020/original/2015-315-FA/15CCT02_SiteInformation/15CCT02_SiteInformation.xlsx
+++ b/data/primary_studies/Marot_et_al_2020/original/2015-315-FA/15CCT02_SiteInformation/15CCT02_SiteInformation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry/Documents/CCN_GitHub/CCRCN-Data-Library/data/primary_studies/Marot_et_al_2020/original/2015-315-FA/15CCT02_SiteInformation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D6215-70FF-A242-9385-BA6B77CF8E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="14655"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14520" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="15CCT02 SiteInfo" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
   <si>
     <t>Water Quality Parameters</t>
   </si>
@@ -72,9 +78,6 @@
   </si>
   <si>
     <t>Sediment Sample Type Key:</t>
-  </si>
-  <si>
-    <t> 30.37012</t>
   </si>
   <si>
     <t>--</t>
@@ -212,11 +215,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="30" x14ac:knownFonts="1">
     <font>
@@ -934,15 +937,15 @@
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -951,7 +954,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -991,7 +994,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="79" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="87" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1102,13 +1105,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1121,7 +1117,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="145" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1211,53 +1207,53 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="140" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="183">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="177"/>
-    <cellStyle name="20% - Accent1 3" xfId="165"/>
+    <cellStyle name="20% - Accent1 2" xfId="177" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent1 3" xfId="165" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="175"/>
-    <cellStyle name="20% - Accent2 3" xfId="163"/>
+    <cellStyle name="20% - Accent2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="173"/>
-    <cellStyle name="20% - Accent3 3" xfId="161"/>
+    <cellStyle name="20% - Accent3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent3 3" xfId="161" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="171"/>
-    <cellStyle name="20% - Accent4 3" xfId="160"/>
+    <cellStyle name="20% - Accent4 2" xfId="171" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Accent4 3" xfId="160" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="152"/>
-    <cellStyle name="20% - Accent5 3" xfId="158"/>
+    <cellStyle name="20% - Accent5 2" xfId="152" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - Accent5 3" xfId="158" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="168"/>
-    <cellStyle name="20% - Accent6 3" xfId="156"/>
+    <cellStyle name="20% - Accent6 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - Accent6 3" xfId="156" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="176"/>
-    <cellStyle name="40% - Accent1 3" xfId="164"/>
+    <cellStyle name="40% - Accent1 2" xfId="176" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40% - Accent1 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="174"/>
-    <cellStyle name="40% - Accent2 3" xfId="162"/>
+    <cellStyle name="40% - Accent2 2" xfId="174" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="40% - Accent2 3" xfId="162" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="172"/>
-    <cellStyle name="40% - Accent3 3" xfId="181"/>
+    <cellStyle name="40% - Accent3 2" xfId="172" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="40% - Accent3 3" xfId="181" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="170"/>
-    <cellStyle name="40% - Accent4 3" xfId="159"/>
+    <cellStyle name="40% - Accent4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="40% - Accent4 3" xfId="159" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="169"/>
-    <cellStyle name="40% - Accent5 3" xfId="157"/>
+    <cellStyle name="40% - Accent5 2" xfId="169" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="40% - Accent5 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="167"/>
-    <cellStyle name="40% - Accent6 3" xfId="155"/>
+    <cellStyle name="40% - Accent6 2" xfId="167" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="40% - Accent6 3" xfId="155" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
@@ -1283,124 +1279,124 @@
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="50"/>
-    <cellStyle name="Normal 100" xfId="140"/>
-    <cellStyle name="Normal 101" xfId="141"/>
-    <cellStyle name="Normal 102" xfId="142"/>
-    <cellStyle name="Normal 103" xfId="143"/>
-    <cellStyle name="Normal 104" xfId="144"/>
-    <cellStyle name="Normal 105" xfId="145"/>
-    <cellStyle name="Normal 106" xfId="146"/>
-    <cellStyle name="Normal 107" xfId="147"/>
-    <cellStyle name="Normal 108" xfId="148"/>
-    <cellStyle name="Normal 109" xfId="149"/>
-    <cellStyle name="Normal 11" xfId="51"/>
-    <cellStyle name="Normal 110" xfId="42"/>
-    <cellStyle name="Normal 111" xfId="182"/>
-    <cellStyle name="Normal 12" xfId="52"/>
-    <cellStyle name="Normal 13" xfId="53"/>
-    <cellStyle name="Normal 14" xfId="54"/>
-    <cellStyle name="Normal 15" xfId="55"/>
-    <cellStyle name="Normal 16" xfId="56"/>
-    <cellStyle name="Normal 17" xfId="57"/>
-    <cellStyle name="Normal 18" xfId="58"/>
-    <cellStyle name="Normal 19" xfId="59"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="43"/>
-    <cellStyle name="Normal 20" xfId="60"/>
-    <cellStyle name="Normal 21" xfId="61"/>
-    <cellStyle name="Normal 22" xfId="62"/>
-    <cellStyle name="Normal 23" xfId="63"/>
-    <cellStyle name="Normal 24" xfId="64"/>
-    <cellStyle name="Normal 25" xfId="65"/>
-    <cellStyle name="Normal 26" xfId="66"/>
-    <cellStyle name="Normal 27" xfId="67"/>
-    <cellStyle name="Normal 28" xfId="68"/>
-    <cellStyle name="Normal 29" xfId="69"/>
-    <cellStyle name="Normal 3" xfId="45"/>
-    <cellStyle name="Normal 3 2" xfId="154"/>
-    <cellStyle name="Normal 3 3" xfId="179"/>
-    <cellStyle name="Normal 30" xfId="70"/>
-    <cellStyle name="Normal 31" xfId="71"/>
-    <cellStyle name="Normal 32" xfId="72"/>
-    <cellStyle name="Normal 33" xfId="73"/>
-    <cellStyle name="Normal 34" xfId="74"/>
-    <cellStyle name="Normal 35" xfId="75"/>
-    <cellStyle name="Normal 36" xfId="76"/>
-    <cellStyle name="Normal 37" xfId="77"/>
-    <cellStyle name="Normal 38" xfId="78"/>
-    <cellStyle name="Normal 39" xfId="79"/>
-    <cellStyle name="Normal 4" xfId="44"/>
-    <cellStyle name="Normal 4 2" xfId="151"/>
-    <cellStyle name="Normal 40" xfId="80"/>
-    <cellStyle name="Normal 41" xfId="81"/>
-    <cellStyle name="Normal 42" xfId="82"/>
-    <cellStyle name="Normal 43" xfId="83"/>
-    <cellStyle name="Normal 44" xfId="84"/>
-    <cellStyle name="Normal 45" xfId="85"/>
-    <cellStyle name="Normal 46" xfId="86"/>
-    <cellStyle name="Normal 47" xfId="87"/>
-    <cellStyle name="Normal 48" xfId="88"/>
-    <cellStyle name="Normal 49" xfId="89"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 5 2" xfId="153"/>
-    <cellStyle name="Normal 50" xfId="90"/>
-    <cellStyle name="Normal 51" xfId="91"/>
-    <cellStyle name="Normal 52" xfId="92"/>
-    <cellStyle name="Normal 53" xfId="93"/>
-    <cellStyle name="Normal 54" xfId="94"/>
-    <cellStyle name="Normal 55" xfId="95"/>
-    <cellStyle name="Normal 56" xfId="96"/>
-    <cellStyle name="Normal 57" xfId="97"/>
-    <cellStyle name="Normal 58" xfId="98"/>
-    <cellStyle name="Normal 59" xfId="99"/>
-    <cellStyle name="Normal 6" xfId="150"/>
-    <cellStyle name="Normal 60" xfId="100"/>
-    <cellStyle name="Normal 61" xfId="101"/>
-    <cellStyle name="Normal 62" xfId="102"/>
-    <cellStyle name="Normal 63" xfId="103"/>
-    <cellStyle name="Normal 64" xfId="104"/>
-    <cellStyle name="Normal 65" xfId="105"/>
-    <cellStyle name="Normal 66" xfId="106"/>
-    <cellStyle name="Normal 67" xfId="107"/>
-    <cellStyle name="Normal 68" xfId="108"/>
-    <cellStyle name="Normal 69" xfId="109"/>
-    <cellStyle name="Normal 7" xfId="47"/>
-    <cellStyle name="Normal 70" xfId="110"/>
-    <cellStyle name="Normal 71" xfId="111"/>
-    <cellStyle name="Normal 72" xfId="112"/>
-    <cellStyle name="Normal 73" xfId="113"/>
-    <cellStyle name="Normal 74" xfId="114"/>
-    <cellStyle name="Normal 75" xfId="115"/>
-    <cellStyle name="Normal 76" xfId="116"/>
-    <cellStyle name="Normal 77" xfId="117"/>
-    <cellStyle name="Normal 78" xfId="118"/>
-    <cellStyle name="Normal 79" xfId="119"/>
-    <cellStyle name="Normal 8" xfId="48"/>
-    <cellStyle name="Normal 80" xfId="120"/>
-    <cellStyle name="Normal 81" xfId="121"/>
-    <cellStyle name="Normal 82" xfId="122"/>
-    <cellStyle name="Normal 83" xfId="123"/>
-    <cellStyle name="Normal 84" xfId="124"/>
-    <cellStyle name="Normal 85" xfId="125"/>
-    <cellStyle name="Normal 86" xfId="126"/>
-    <cellStyle name="Normal 87" xfId="127"/>
-    <cellStyle name="Normal 88" xfId="128"/>
-    <cellStyle name="Normal 89" xfId="129"/>
-    <cellStyle name="Normal 9" xfId="49"/>
-    <cellStyle name="Normal 90" xfId="130"/>
-    <cellStyle name="Normal 91" xfId="131"/>
-    <cellStyle name="Normal 92" xfId="132"/>
-    <cellStyle name="Normal 93" xfId="133"/>
-    <cellStyle name="Normal 94" xfId="134"/>
-    <cellStyle name="Normal 95" xfId="135"/>
-    <cellStyle name="Normal 96" xfId="136"/>
-    <cellStyle name="Normal 97" xfId="137"/>
-    <cellStyle name="Normal 98" xfId="138"/>
-    <cellStyle name="Normal 99" xfId="139"/>
-    <cellStyle name="Note 2" xfId="180"/>
-    <cellStyle name="Note 3" xfId="178"/>
-    <cellStyle name="Note 4" xfId="166"/>
+    <cellStyle name="Normal 10" xfId="50" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 100" xfId="140" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 101" xfId="141" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 102" xfId="142" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 103" xfId="143" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 104" xfId="144" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 105" xfId="145" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 106" xfId="146" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 107" xfId="147" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 108" xfId="148" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 109" xfId="149" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 11" xfId="51" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 110" xfId="42" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 111" xfId="182" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 12" xfId="52" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 13" xfId="53" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 14" xfId="54" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 15" xfId="55" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 16" xfId="56" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 17" xfId="57" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 18" xfId="58" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 19" xfId="59" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 2 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 20" xfId="60" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 21" xfId="61" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 22" xfId="62" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 23" xfId="63" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 24" xfId="64" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 25" xfId="65" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 26" xfId="66" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 27" xfId="67" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 28" xfId="68" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 29" xfId="69" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 3 2" xfId="154" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 3 3" xfId="179" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 30" xfId="70" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 31" xfId="71" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 32" xfId="72" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 33" xfId="73" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 34" xfId="74" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 35" xfId="75" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 36" xfId="76" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 37" xfId="77" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 38" xfId="78" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 39" xfId="79" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 4" xfId="44" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 4 2" xfId="151" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 40" xfId="80" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 41" xfId="81" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 42" xfId="82" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 43" xfId="83" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 44" xfId="84" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 45" xfId="85" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 46" xfId="86" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 47" xfId="87" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 48" xfId="88" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 49" xfId="89" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 5 2" xfId="153" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 50" xfId="90" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 51" xfId="91" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 52" xfId="92" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 53" xfId="93" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 54" xfId="94" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 55" xfId="95" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 56" xfId="96" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 57" xfId="97" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 58" xfId="98" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 59" xfId="99" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 6" xfId="150" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 60" xfId="100" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 61" xfId="101" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 62" xfId="102" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 63" xfId="103" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 64" xfId="104" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 65" xfId="105" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 66" xfId="106" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 67" xfId="107" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 68" xfId="108" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 69" xfId="109" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 7" xfId="47" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 70" xfId="110" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 71" xfId="111" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 72" xfId="112" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 73" xfId="113" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 74" xfId="114" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 75" xfId="115" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 76" xfId="116" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 77" xfId="117" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 78" xfId="118" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 79" xfId="119" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 8" xfId="48" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 80" xfId="120" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 81" xfId="121" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 82" xfId="122" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 83" xfId="123" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 84" xfId="124" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 85" xfId="125" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 86" xfId="126" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 87" xfId="127" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 88" xfId="128" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 89" xfId="129" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 9" xfId="49" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 90" xfId="130" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 91" xfId="131" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Normal 92" xfId="132" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Normal 93" xfId="133" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Normal 94" xfId="134" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Normal 95" xfId="135" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Normal 96" xfId="136" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Normal 97" xfId="137" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Normal 98" xfId="138" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Normal 99" xfId="139" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Note 2" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Note 3" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Note 4" xfId="166" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -1411,6 +1407,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1459,7 +1458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1492,9 +1491,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1527,6 +1543,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1702,66 +1735,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="12.42578125" style="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="1" customWidth="1"/>
-    <col min="8" max="12" width="13.28515625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="12.42578125" style="1"/>
-    <col min="15" max="15" width="16.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="12.42578125" style="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="12.5" style="1"/>
+    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="1" customWidth="1"/>
+    <col min="8" max="12" width="13.33203125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="12.5" style="1"/>
+    <col min="15" max="15" width="16.5" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="12.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-    </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="94" t="s">
+    <row r="1" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2"/>
+      <c r="H2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-    </row>
-    <row r="3" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+    </row>
+    <row r="3" spans="1:18" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1803,26 +1836,26 @@
         <v>6</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="96">
+        <v>29</v>
+      </c>
+      <c r="B4" s="91">
         <v>42154</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="62">
         <v>30.35998</v>
       </c>
-      <c r="E4" s="66">
+      <c r="E4" s="63">
         <v>-88.368070000000003</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="32">
         <v>3.1</v>
       </c>
       <c r="G4" s="55"/>
@@ -1851,20 +1884,20 @@
         <v>183.5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="96">
+        <v>30</v>
+      </c>
+      <c r="B5" s="91">
         <v>42154</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="68">
+      <c r="D5" s="64">
+        <v>30.37012</v>
+      </c>
+      <c r="E5" s="65">
         <v>-88.358630000000005</v>
       </c>
       <c r="F5" s="32">
@@ -1896,23 +1929,23 @@
         <v>136.30000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="96">
+        <v>31</v>
+      </c>
+      <c r="B6" s="91">
         <v>42154</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="69">
+      <c r="D6" s="66">
         <v>30.362069999999999</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="67">
         <v>-88.348669999999998</v>
       </c>
-      <c r="F6" s="58">
+      <c r="F6" s="32">
         <v>3</v>
       </c>
       <c r="G6" s="55"/>
@@ -1941,20 +1974,20 @@
         <v>114.5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="96">
+        <v>32</v>
+      </c>
+      <c r="B7" s="91">
         <v>42154</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="68">
         <v>30.366479999999999</v>
       </c>
-      <c r="E7" s="72">
+      <c r="E7" s="69">
         <v>-88.331180000000003</v>
       </c>
       <c r="F7" s="32">
@@ -1970,8 +2003,8 @@
       <c r="J7" s="32">
         <v>85.5</v>
       </c>
-      <c r="K7" s="61" t="s">
-        <v>20</v>
+      <c r="K7" s="58" t="s">
+        <v>19</v>
       </c>
       <c r="L7" s="31">
         <v>24.96</v>
@@ -1986,20 +2019,20 @@
         <v>119.2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="96">
+        <v>33</v>
+      </c>
+      <c r="B8" s="91">
         <v>42154</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="70">
         <v>30.379280000000001</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="71">
         <v>-88.322515999999993</v>
       </c>
       <c r="F8" s="32">
@@ -2031,20 +2064,20 @@
         <v>126.8</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="96">
+        <v>34</v>
+      </c>
+      <c r="B9" s="91">
         <v>42155</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="72">
         <v>30.38203</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="73">
         <v>-88.344530000000006</v>
       </c>
       <c r="F9" s="32">
@@ -2076,20 +2109,20 @@
         <v>137.5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="96">
+        <v>35</v>
+      </c>
+      <c r="B10" s="91">
         <v>42155</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="74">
         <v>30.376729999999998</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="75">
         <v>-88.36403</v>
       </c>
       <c r="F10" s="32">
@@ -2111,7 +2144,7 @@
       <c r="L10" s="15">
         <v>20.89</v>
       </c>
-      <c r="M10" s="59">
+      <c r="M10" s="15">
         <v>12.42</v>
       </c>
       <c r="N10" s="15">
@@ -2124,20 +2157,20 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="96">
+        <v>36</v>
+      </c>
+      <c r="B11" s="91">
         <v>42155</v>
       </c>
       <c r="C11" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="79">
+      <c r="D11" s="76">
         <v>30.392060000000001</v>
       </c>
-      <c r="E11" s="80">
+      <c r="E11" s="77">
         <v>-88.373440000000002</v>
       </c>
       <c r="F11" s="32">
@@ -2169,20 +2202,20 @@
         <v>126.1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="96">
+        <v>37</v>
+      </c>
+      <c r="B12" s="91">
         <v>42156</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="81">
+      <c r="D12" s="78">
         <v>30.379519999999999</v>
       </c>
-      <c r="E12" s="82">
+      <c r="E12" s="79">
         <v>-88.379469999999998</v>
       </c>
       <c r="F12" s="32">
@@ -2214,11 +2247,11 @@
         <v>114.1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="96">
+        <v>38</v>
+      </c>
+      <c r="B13" s="91">
         <v>42156</v>
       </c>
       <c r="C13" s="33" t="s">
@@ -2227,7 +2260,7 @@
       <c r="D13" s="10">
         <v>30.356839999999998</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="80">
         <v>-88.344210000000004</v>
       </c>
       <c r="F13" s="32">
@@ -2259,20 +2292,20 @@
         <v>121.9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="96">
+        <v>39</v>
+      </c>
+      <c r="B14" s="91">
         <v>42156</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="84">
+      <c r="D14" s="81">
         <v>30.361599999999999</v>
       </c>
-      <c r="E14" s="85">
+      <c r="E14" s="82">
         <v>-88.325739999999996</v>
       </c>
       <c r="F14" s="32">
@@ -2304,11 +2337,11 @@
         <v>131.6</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="96">
+        <v>41</v>
+      </c>
+      <c r="B15" s="91">
         <v>42156</v>
       </c>
       <c r="C15" s="33" t="s">
@@ -2349,11 +2382,11 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="96">
+        <v>40</v>
+      </c>
+      <c r="B16" s="91">
         <v>42156</v>
       </c>
       <c r="C16" s="33" t="s">
@@ -2394,11 +2427,11 @@
         <v>87.3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="96">
+        <v>42</v>
+      </c>
+      <c r="B17" s="91">
         <v>42156</v>
       </c>
       <c r="C17" s="33" t="s">
@@ -2439,11 +2472,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="96">
+        <v>43</v>
+      </c>
+      <c r="B18" s="91">
         <v>42156</v>
       </c>
       <c r="C18" s="33" t="s">
@@ -2484,11 +2517,11 @@
         <v>78.400000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="96">
+        <v>44</v>
+      </c>
+      <c r="B19" s="91">
         <v>42157</v>
       </c>
       <c r="C19" s="33" t="s">
@@ -2529,11 +2562,11 @@
         <v>180.2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="96">
+        <v>45</v>
+      </c>
+      <c r="B20" s="91">
         <v>42157</v>
       </c>
       <c r="C20" s="33" t="s">
@@ -2574,11 +2607,11 @@
         <v>176.3</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="96">
+        <v>46</v>
+      </c>
+      <c r="B21" s="91">
         <v>42157</v>
       </c>
       <c r="C21" s="33" t="s">
@@ -2587,7 +2620,7 @@
       <c r="D21" s="18">
         <v>30.39162</v>
       </c>
-      <c r="E21" s="86">
+      <c r="E21" s="83">
         <v>-88.350880000000004</v>
       </c>
       <c r="F21" s="32">
@@ -2619,11 +2652,11 @@
         <v>157.19999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="96">
+        <v>47</v>
+      </c>
+      <c r="B22" s="91">
         <v>42158</v>
       </c>
       <c r="C22" s="33" t="s">
@@ -2632,7 +2665,7 @@
       <c r="D22" s="23">
         <v>30.372479999999999</v>
       </c>
-      <c r="E22" s="87">
+      <c r="E22" s="84">
         <v>-88.393940000000001</v>
       </c>
       <c r="F22" s="32">
@@ -2664,11 +2697,11 @@
         <v>109.1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="96">
+        <v>48</v>
+      </c>
+      <c r="B23" s="91">
         <v>42158</v>
       </c>
       <c r="C23" s="33" t="s">
@@ -2709,11 +2742,11 @@
         <v>103.7</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="96">
+        <v>49</v>
+      </c>
+      <c r="B24" s="91">
         <v>42158</v>
       </c>
       <c r="C24" s="33" t="s">
@@ -2754,20 +2787,20 @@
         <v>106.7</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="96">
+        <v>50</v>
+      </c>
+      <c r="B25" s="91">
         <v>42158</v>
       </c>
       <c r="C25" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="88">
+      <c r="D25" s="85">
         <v>30.40981</v>
       </c>
-      <c r="E25" s="89">
+      <c r="E25" s="86">
         <v>-88.402500000000003</v>
       </c>
       <c r="F25" s="32">
@@ -2799,11 +2832,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="96">
+        <v>51</v>
+      </c>
+      <c r="B26" s="91">
         <v>42158</v>
       </c>
       <c r="C26" s="33" t="s">
@@ -2812,27 +2845,27 @@
       <c r="D26" s="44">
         <v>30.3947</v>
       </c>
-      <c r="E26" s="90">
+      <c r="E26" s="87">
         <v>-88.399820000000005</v>
       </c>
       <c r="F26" s="32">
         <v>3</v>
       </c>
       <c r="G26" s="6"/>
-      <c r="H26" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="60" t="s">
-        <v>20</v>
+      <c r="H26" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="57" t="s">
+        <v>19</v>
       </c>
       <c r="M26" s="31">
         <v>12</v>
@@ -2841,14 +2874,14 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="O26" s="32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="96">
+        <v>52</v>
+      </c>
+      <c r="B27" s="91">
         <v>42157</v>
       </c>
       <c r="C27" s="33" t="s">
@@ -2889,11 +2922,11 @@
         <v>138.1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="96">
+        <v>53</v>
+      </c>
+      <c r="B28" s="91">
         <v>42158</v>
       </c>
       <c r="C28" s="33" t="s">
@@ -2902,7 +2935,7 @@
       <c r="D28" s="41">
         <v>30.40042</v>
       </c>
-      <c r="E28" s="91">
+      <c r="E28" s="88">
         <v>-88.39828</v>
       </c>
       <c r="F28" s="32">
@@ -2934,11 +2967,11 @@
         <v>128.9</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="96">
+        <v>60</v>
+      </c>
+      <c r="B29" s="91">
         <v>42153</v>
       </c>
       <c r="C29" s="33" t="s">
@@ -2979,11 +3012,11 @@
         <v>189.4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="96">
+        <v>54</v>
+      </c>
+      <c r="B30" s="91">
         <v>42157</v>
       </c>
       <c r="C30" s="33" t="s">
@@ -3024,11 +3057,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="96">
+        <v>55</v>
+      </c>
+      <c r="B31" s="91">
         <v>42153</v>
       </c>
       <c r="C31" s="33" t="s">
@@ -3069,11 +3102,11 @@
         <v>147.5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="96">
+        <v>56</v>
+      </c>
+      <c r="B32" s="91">
         <v>42157</v>
       </c>
       <c r="C32" s="33" t="s">
@@ -3082,7 +3115,7 @@
       <c r="D32" s="46">
         <v>30.374479999999998</v>
       </c>
-      <c r="E32" s="92">
+      <c r="E32" s="89">
         <v>-88.39228</v>
       </c>
       <c r="F32" s="32">
@@ -3114,11 +3147,11 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="96">
+        <v>57</v>
+      </c>
+      <c r="B33" s="91">
         <v>42155</v>
       </c>
       <c r="C33" s="33" t="s">
@@ -3159,11 +3192,11 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="96">
+        <v>58</v>
+      </c>
+      <c r="B34" s="91">
         <v>42155</v>
       </c>
       <c r="C34" s="33" t="s">
@@ -3204,11 +3237,11 @@
         <v>116.3</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="96">
+        <v>59</v>
+      </c>
+      <c r="B35" s="91">
         <v>42154</v>
       </c>
       <c r="C35" s="33" t="s">
@@ -3249,11 +3282,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="96">
+        <v>24</v>
+      </c>
+      <c r="B36" s="91">
         <v>42153</v>
       </c>
       <c r="C36" s="33" t="s">
@@ -3262,7 +3295,7 @@
       <c r="D36" s="34">
         <v>30.376529999999999</v>
       </c>
-      <c r="E36" s="93">
+      <c r="E36" s="90">
         <v>-88.390720000000002</v>
       </c>
       <c r="F36" s="33">
@@ -3270,35 +3303,35 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K36" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L36" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M36" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N36" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O36" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="96">
+        <v>25</v>
+      </c>
+      <c r="B37" s="91">
         <v>42153</v>
       </c>
       <c r="C37" s="33" t="s">
@@ -3315,44 +3348,44 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K37" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L37" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M37" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N37" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="96">
+        <v>26</v>
+      </c>
+      <c r="B38" s="91">
         <v>42153</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="59">
         <v>30.376670000000001</v>
       </c>
-      <c r="E38" s="63">
+      <c r="E38" s="60">
         <v>-88.39076</v>
       </c>
       <c r="F38" s="33">
@@ -3360,44 +3393,44 @@
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J38" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K38" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L38" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M38" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N38" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O38" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="96">
+        <v>27</v>
+      </c>
+      <c r="B39" s="91">
         <v>42158</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="64">
+      <c r="D39" s="61">
         <v>30.417761111111101</v>
       </c>
-      <c r="E39" s="64">
+      <c r="E39" s="61">
         <v>-88.405522222222203</v>
       </c>
       <c r="F39" s="32">
@@ -3428,51 +3461,51 @@
         <v>175.3</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="96">
+        <v>28</v>
+      </c>
+      <c r="B40" s="91">
         <v>42158</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="64">
+      <c r="D40" s="61">
         <v>30.4174583333333</v>
       </c>
-      <c r="E40" s="64">
+      <c r="E40" s="61">
         <v>-88.405372222222198</v>
       </c>
       <c r="F40" s="32">
         <v>0</v>
       </c>
-      <c r="H40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="I40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="J40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="K40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="M40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="N40" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="O40" s="60" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="N40" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="O40" s="57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="56" t="s">
         <v>18</v>
       </c>
@@ -3491,9 +3524,9 @@
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
     </row>
-    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42"/>
       <c r="E42"/>
@@ -3508,14 +3541,14 @@
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>